<commit_message>
Add first draft of R code for bias module
Incudes lab warm-up and lab. It still needs to be formatted correctly.
</commit_message>
<xml_diff>
--- a/modules/07 Bias/🔬Lab - Bias.xlsx
+++ b/modules/07 Bias/🔬Lab - Bias.xlsx
@@ -1,61 +1,129 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25809"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_A65844DAEFC1AFBF0418882FCA4798CBCC40CD25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Measurement Error" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sens and Misclass" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Doug" sheetId="3" r:id="rId6"/>
+    <sheet name="Measurement Error" sheetId="1" r:id="rId1"/>
+    <sheet name="Sens and Misclass" sheetId="2" r:id="rId2"/>
+    <sheet name="Doug" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="B5">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
-        <t xml:space="preserve">The proportion of people with disease who test positive.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The proportion of people with disease who test positive.</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C5">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
-        <t xml:space="preserve">The proportion of people without the disease who test negative.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The proportion of people without the disease who test negative.</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A8">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
-        <t xml:space="preserve">Numbers from Exhibit 4-3 in Szklo</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Numbers from Exhibit 4-3 in Szklo</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A16">
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
-        <t xml:space="preserve">Among those with disease, we correctly classified 90% who were exposed as being exposed. We incorrectly classified 10% who were exposed as being unexposed.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Among those with disease, we correctly classified 90% who were exposed as being exposed. We incorrectly classified 10% who were exposed as being unexposed.</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A17">
+    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
-        <t xml:space="preserve">Among those with disease, we correctly classified 80% who were unexposed as being unexposed. We incorrectly classified 20% who were unexposed as being exposed.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Among those with disease, we correctly classified 80% who were unexposed as being unexposed. We incorrectly classified 20% who were unexposed as being exposed.</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A18">
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
-        <t xml:space="preserve">Among those without disease, we correctly classified 90% who were exposed as being exposed. We incorrectly classified 10% who were exposed as being unexposed.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Among those without disease, we correctly classified 90% who were exposed as being exposed. We incorrectly classified 10% who were exposed as being unexposed.</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A19">
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
-        <t xml:space="preserve">Among those without disease, we correctly classified 80% who were unexposed as being unexposed. We incorrectly classified 20% who were unexposed as being exposed.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Among those without disease, we correctly classified 80% who were unexposed as being unexposed. We incorrectly classified 20% who were unexposed as being exposed.</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A21">
+    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
-        <t xml:space="preserve">Numbers from Exhibit 4-3 in Szklo</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Numbers from Exhibit 4-3 in Szklo</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -218,20 +286,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
@@ -241,7 +311,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -263,59 +333,51 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -505,26 +567,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.5"/>
-    <col customWidth="1" min="2" max="2" width="16.5"/>
-    <col customWidth="1" min="3" max="3" width="14.13"/>
-    <col customWidth="1" min="4" max="4" width="15.63"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,505 +603,512 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
-        <v>146.0</v>
+        <v>146</v>
       </c>
       <c r="B2" s="1">
-        <v>136.0</v>
-      </c>
-      <c r="C2" s="3">
-        <f t="shared" ref="C2:D2" si="1">A2+5</f>
+        <v>136</v>
+      </c>
+      <c r="C2" s="1">
+        <f t="shared" ref="C2:D2" si="0">A2+5</f>
         <v>151</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
+        <f t="shared" si="0"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
+        <v>147</v>
+      </c>
+      <c r="B3" s="1">
+        <v>137</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:D3" si="1">A3+5</f>
+        <v>152</v>
+      </c>
+      <c r="D3" s="1">
         <f t="shared" si="1"/>
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>147.0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>137.0</v>
-      </c>
-      <c r="C3" s="3">
-        <f t="shared" ref="C3:D3" si="2">A3+5</f>
-        <v>152</v>
-      </c>
-      <c r="D3" s="3">
-        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
-        <v>148.0</v>
+        <v>148</v>
       </c>
       <c r="B4" s="1">
-        <v>138.0</v>
-      </c>
-      <c r="C4" s="3">
-        <f t="shared" ref="C4:D4" si="3">A4+5</f>
+        <v>138</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:D4" si="2">A4+5</f>
         <v>153</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>149</v>
+      </c>
+      <c r="B5" s="1">
+        <v>139</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:D5" si="3">A5+5</f>
+        <v>154</v>
+      </c>
+      <c r="D5" s="1">
         <f t="shared" si="3"/>
-        <v>143</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>149.0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>139.0</v>
-      </c>
-      <c r="C5" s="3">
-        <f t="shared" ref="C5:D5" si="4">A5+5</f>
-        <v>154</v>
-      </c>
-      <c r="D5" s="3">
-        <f t="shared" si="4"/>
         <v>144</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <f>AVERAGE(A2:A11)</f>
         <v>150</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <f>AVERAGE(A2:A11)</f>
         <v>150</v>
       </c>
-      <c r="I5" s="5">
-        <f t="shared" ref="I5:I7" si="6">G5-H5</f>
+      <c r="I5" s="3">
+        <f t="shared" ref="I5:I7" si="4">G5-H5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="B6" s="1">
-        <v>140.0</v>
-      </c>
-      <c r="C6" s="3">
+        <v>140</v>
+      </c>
+      <c r="C6" s="1">
         <f t="shared" ref="C6:D6" si="5">A6+5</f>
         <v>155</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <f t="shared" si="5"/>
         <v>145</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <f>AVERAGE(B2:B11)</f>
         <v>140</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <f>AVERAGE(B2:B11)</f>
         <v>140</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>150</v>
+      </c>
+      <c r="B7" s="1">
+        <v>140</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" ref="C7:D7" si="6">A7+5</f>
+        <v>155</v>
+      </c>
+      <c r="D7" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1">
-        <v>150.0</v>
-      </c>
-      <c r="B7" s="1">
-        <v>140.0</v>
-      </c>
-      <c r="C7" s="3">
-        <f t="shared" ref="C7:D7" si="7">A7+5</f>
-        <v>155</v>
-      </c>
-      <c r="D7" s="3">
-        <f t="shared" si="7"/>
         <v>145</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="5">
-        <f t="shared" ref="G7:H7" si="8">G5-G6</f>
+      <c r="G7" s="3">
+        <f t="shared" ref="G7:H7" si="7">G5-G6</f>
         <v>10</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1">
+        <v>151</v>
+      </c>
+      <c r="B8" s="1">
+        <v>141</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ref="C8:D8" si="8">A8+5</f>
+        <v>156</v>
+      </c>
+      <c r="D8" s="1">
         <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="I7" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1">
-        <v>151.0</v>
-      </c>
-      <c r="B8" s="1">
-        <v>141.0</v>
-      </c>
-      <c r="C8" s="3">
-        <f t="shared" ref="C8:D8" si="9">A8+5</f>
-        <v>156</v>
-      </c>
-      <c r="D8" s="3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1">
+        <v>152</v>
+      </c>
+      <c r="B9" s="1">
+        <v>142</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" ref="C9:D9" si="9">A9+5</f>
+        <v>157</v>
+      </c>
+      <c r="D9" s="1">
         <f t="shared" si="9"/>
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1">
-        <v>152.0</v>
-      </c>
-      <c r="B9" s="1">
-        <v>142.0</v>
-      </c>
-      <c r="C9" s="3">
-        <f t="shared" ref="C9:D9" si="10">A9+5</f>
-        <v>157</v>
-      </c>
-      <c r="D9" s="3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>153</v>
+      </c>
+      <c r="B10" s="1">
+        <v>143</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" ref="C10:D10" si="10">A10+5</f>
+        <v>158</v>
+      </c>
+      <c r="D10" s="1">
         <f t="shared" si="10"/>
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1">
-        <v>153.0</v>
-      </c>
-      <c r="B10" s="1">
-        <v>143.0</v>
-      </c>
-      <c r="C10" s="3">
-        <f t="shared" ref="C10:D10" si="11">A10+5</f>
-        <v>158</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="11"/>
         <v>148</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
-        <v>154.0</v>
+        <v>154</v>
       </c>
       <c r="B11" s="1">
-        <v>144.0</v>
-      </c>
-      <c r="C11" s="3">
-        <f t="shared" ref="C11:D11" si="12">A11+5</f>
+        <v>144</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" ref="C11:D11" si="11">A11+5</f>
         <v>159</v>
       </c>
-      <c r="D11" s="3">
-        <f t="shared" si="12"/>
+      <c r="D11" s="1">
+        <f t="shared" si="11"/>
         <v>149</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9">
       <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="3">
         <f>AVERAGE(A2:A11)</f>
         <v>150</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="3">
         <f>AVERAGE(C2:C11)</f>
         <v>155</v>
       </c>
-      <c r="I12" s="5">
-        <f t="shared" ref="I12:I14" si="13">G12-H12</f>
+      <c r="I12" s="3">
+        <f t="shared" ref="I12:I14" si="12">G12-H12</f>
         <v>-5</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9">
       <c r="F13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="3">
         <f>AVERAGE(B2:B11)</f>
         <v>140</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="3">
         <f>AVERAGE(D2:D11)</f>
         <v>145</v>
       </c>
-      <c r="I13" s="5">
-        <f t="shared" si="13"/>
+      <c r="I13" s="3">
+        <f t="shared" si="12"/>
         <v>-5</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9">
       <c r="F14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="5">
-        <f t="shared" ref="G14:H14" si="14">G12-G13</f>
+      <c r="G14" s="3">
+        <f t="shared" ref="G14:H14" si="13">G12-G13</f>
         <v>10</v>
       </c>
-      <c r="H14" s="5">
-        <f t="shared" si="14"/>
+      <c r="H14" s="3">
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
-      <c r="I14" s="5">
-        <f t="shared" si="13"/>
+      <c r="I14" s="3">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="6:9">
       <c r="F17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18">
-      <c r="F18" s="4" t="s">
+    <row r="18" spans="6:9">
+      <c r="F18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="6:9">
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="3">
         <f>AVERAGE(A2:A11)</f>
         <v>150</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="3">
         <f>AVERAGE(C2:C11)</f>
         <v>155</v>
       </c>
-      <c r="I19" s="5">
-        <f t="shared" ref="I19:I21" si="15">G19-H19</f>
+      <c r="I19" s="3">
+        <f t="shared" ref="I19:I21" si="14">G19-H19</f>
         <v>-5</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="6:9">
       <c r="F20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="3">
         <f>AVERAGE(B2:B11)</f>
         <v>140</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="3">
         <f>AVERAGE(B2:B11)</f>
         <v>140</v>
       </c>
-      <c r="I20" s="5">
-        <f t="shared" si="15"/>
+      <c r="I20" s="3">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="6:9">
       <c r="F21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="5">
-        <f t="shared" ref="G21:H21" si="16">G19-G20</f>
+      <c r="G21" s="3">
+        <f t="shared" ref="G21:H21" si="15">G19-G20</f>
         <v>10</v>
       </c>
-      <c r="H21" s="5">
-        <f t="shared" si="16"/>
+      <c r="H21" s="3">
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
-      <c r="I21" s="5">
-        <f t="shared" si="15"/>
+      <c r="I21" s="3">
+        <f t="shared" si="14"/>
         <v>-5</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="17.5"/>
-    <col customWidth="1" min="3" max="3" width="20.13"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="B2" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:4">
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="4" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4">
-        <v>80.0</v>
-      </c>
-      <c r="C10" s="4">
-        <v>50.0</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" ref="D10:D12" si="1">B10+C10</f>
+      <c r="B10" s="3">
+        <v>80</v>
+      </c>
+      <c r="C10" s="3">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" ref="D10:D12" si="0">B10+C10</f>
         <v>130</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4">
-        <v>20.0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>50.0</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="B11" s="3">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="3">
+        <f t="shared" ref="B12:C12" si="1">B10+B11</f>
+        <v>100</v>
+      </c>
+      <c r="C12" s="3">
         <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="5">
-        <f t="shared" ref="B12:C12" si="2">B10+B11</f>
         <v>100</v>
       </c>
-      <c r="C12" s="5">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" si="1"/>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5">
-        <f t="shared" ref="B13:C13" si="3">B10/B11</f>
+      <c r="B13" s="3">
+        <f t="shared" ref="B13:C13" si="2">B10/B11</f>
         <v>4</v>
       </c>
-      <c r="C13" s="5">
-        <f t="shared" si="3"/>
+      <c r="C13" s="3">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="3">
         <f>B13/C13</f>
         <v>4</v>
       </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="16">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1044,7 +1116,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1052,7 +1124,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1060,7 +1132,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1068,430 +1140,447 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:4">
+      <c r="A21" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="8" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="B23" s="4" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="B23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="4">
-        <f t="shared" ref="B24:B25" si="4">B10*D16</f>
+      <c r="B24" s="3">
+        <f t="shared" ref="B24:B25" si="3">B10*D16</f>
         <v>72</v>
       </c>
-      <c r="C24" s="4">
-        <f t="shared" ref="C24:C25" si="5">C10*D18</f>
+      <c r="C24" s="3">
+        <f t="shared" ref="C24:C25" si="4">C10*D18</f>
         <v>45</v>
       </c>
-      <c r="D24" s="3">
-        <f t="shared" ref="D24:D26" si="6">B24+C24</f>
+      <c r="D24" s="1">
+        <f t="shared" ref="D24:D26" si="5">B24+C24</f>
         <v>117</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="C25" s="3">
         <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="C25" s="4">
+        <v>40</v>
+      </c>
+      <c r="D25" s="1">
         <f t="shared" si="5"/>
-        <v>40</v>
-      </c>
-      <c r="D25" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="B26" s="3">
+        <f t="shared" ref="B26:C26" si="6">B24+B25</f>
+        <v>88</v>
+      </c>
+      <c r="C26" s="3">
         <f t="shared" si="6"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" s="5">
-        <f t="shared" ref="B26:C26" si="7">B24+B25</f>
-        <v>88</v>
-      </c>
-      <c r="C26" s="5">
-        <f t="shared" si="7"/>
         <v>85</v>
       </c>
-      <c r="D26" s="3">
-        <f t="shared" si="6"/>
+      <c r="D26" s="1">
+        <f t="shared" si="5"/>
         <v>173</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="5">
-        <f t="shared" ref="B27:C27" si="8">B24/B25</f>
+      <c r="B27" s="3">
+        <f t="shared" ref="B27:C27" si="7">B24/B25</f>
         <v>4.5</v>
       </c>
-      <c r="C27" s="5">
-        <f t="shared" si="8"/>
+      <c r="C27" s="3">
+        <f t="shared" si="7"/>
         <v>1.125</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="3">
         <f>B27/C27</f>
         <v>4</v>
       </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="8" t="s">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="B31" s="4" t="s">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="B31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="4">
-        <f t="shared" ref="B32:C32" si="9">B11-B25</f>
+      <c r="B32" s="3">
+        <f t="shared" ref="B32:C32" si="8">B11-B25</f>
         <v>4</v>
       </c>
-      <c r="C32" s="4">
-        <f t="shared" si="9"/>
+      <c r="C32" s="3">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="D32" s="3">
-        <f t="shared" ref="D32:D34" si="11">B32+C32</f>
+      <c r="D32" s="1">
+        <f t="shared" ref="D32:D34" si="9">B32+C32</f>
         <v>14</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <f t="shared" ref="B33:C33" si="10">B10-B24</f>
         <v>8</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="1">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="B34" s="3">
+        <f t="shared" ref="B34:C34" si="11">B32+B33</f>
+        <v>12</v>
+      </c>
+      <c r="C34" s="3">
         <f t="shared" si="11"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" s="5">
-        <f t="shared" ref="B34:C34" si="12">B32+B33</f>
-        <v>12</v>
-      </c>
-      <c r="C34" s="5">
-        <f t="shared" si="12"/>
         <v>15</v>
       </c>
-      <c r="D34" s="3">
-        <f t="shared" si="11"/>
+      <c r="D34" s="1">
+        <f t="shared" si="9"/>
         <v>27</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="B37" s="4" t="s">
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="B37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="4">
-        <f t="shared" ref="B38:C38" si="13">B24+B32</f>
+      <c r="B38" s="3">
+        <f t="shared" ref="B38:C38" si="12">B24+B32</f>
         <v>76</v>
       </c>
-      <c r="C38" s="4">
-        <f t="shared" si="13"/>
+      <c r="C38" s="3">
+        <f t="shared" si="12"/>
         <v>55</v>
       </c>
-      <c r="D38" s="3">
-        <f t="shared" ref="D38:D40" si="15">B38+C38</f>
+      <c r="D38" s="1">
+        <f t="shared" ref="D38:D40" si="13">B38+C38</f>
         <v>131</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <f t="shared" ref="B39:C39" si="14">B25+B33</f>
         <v>24</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <f t="shared" si="14"/>
         <v>45</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="1">
+        <f t="shared" si="13"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="B40" s="3">
+        <f t="shared" ref="B40:C40" si="15">B38+B39</f>
+        <v>100</v>
+      </c>
+      <c r="C40" s="3">
         <f t="shared" si="15"/>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" s="5">
-        <f t="shared" ref="B40:C40" si="16">B38+B39</f>
         <v>100</v>
       </c>
-      <c r="C40" s="5">
-        <f t="shared" si="16"/>
-        <v>100</v>
-      </c>
-      <c r="D40" s="3">
-        <f t="shared" si="15"/>
+      <c r="D40" s="1">
+        <f t="shared" si="13"/>
         <v>200</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="5">
-        <f t="shared" ref="B41:C41" si="17">B38/B39</f>
-        <v>3.166666667</v>
-      </c>
-      <c r="C41" s="5">
-        <f t="shared" si="17"/>
-        <v>1.222222222</v>
-      </c>
-    </row>
-    <row r="42">
+      <c r="B41" s="3">
+        <f t="shared" ref="B41:C41" si="16">B38/B39</f>
+        <v>3.1666666669999999</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="16"/>
+        <v>1.2222222220000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="3">
         <f>B41/C41</f>
-        <v>2.590909091</v>
-      </c>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="44">
+        <v>2.5909090909999999</v>
+      </c>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A36:D36"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A36:D36"/>
   </mergeCells>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.5"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:5">
+      <c r="B1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="B2" s="4" t="s">
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:5">
+      <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="4" t="s">
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -1503,7 +1592,7 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:E14"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
 
@@ -1731,15 +1820,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e3793ca1-6164-4dfb-aaf8-0aa60c0c70c2">
@@ -1750,14 +1830,23 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B5B5E69-2D29-4CEE-8D08-F9C0ABA08B73}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{428C08CE-7399-43C7-8322-72CB72AA8197}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA958F0F-B158-46A3-AC34-40E70DA24BE8}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA958F0F-B158-46A3-AC34-40E70DA24BE8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{428C08CE-7399-43C7-8322-72CB72AA8197}"/>
 </file>
</xml_diff>